<commit_message>
fix(description-summary): fixed the bug in scraping desc summary
</commit_message>
<xml_diff>
--- a/Techversant_Jobs.xlsx
+++ b/Techversant_Jobs.xlsx
@@ -459,7 +459,7 @@
     <col width="58" customWidth="1" min="3" max="3"/>
     <col width="25" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="80" customWidth="1" min="6" max="6"/>
     <col width="80" customWidth="1" min="7" max="7"/>
     <col width="33" customWidth="1" min="8" max="8"/>
     <col width="80" customWidth="1" min="9" max="9"/>
@@ -564,7 +564,42 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Client Engagement &amp; Consulting
+Interact directly with clients and stakeholders to understand complex business problems.
+Translate business needs into AI/ML opportunities and articulate solution strategies clearly.
+Present solution architectures, effort estimates, timelines, and potential ROI.
+Solution Design &amp; Architecture
+Define end-to-end AI architecture including data pipelines, model selection, AI engines, integration layers, APIs, and deployment strategies.
+Make informed choices of AI/ML/DL algorithms, frameworks, and platforms based on problem type and constraints.
+Ensure the architecture is scalable, modular, secure, and optimized for performance.
+Hands-On Development
+Develop critical components or proof-of-concepts when needed.
+Perform hands-on design and coding for pipelines, model training, inferencing, or integrations.
+Create reusable components and automation scripts for repeatability.
+Team Leadership &amp; Delivery Oversight
+Build and mentor a high-performing AI development team.
+Drive agile development cycles, ensuring timely and quality delivery.
+Collaborate with DevOps, Product Managers, and QA teams throughout SDLC.
+Client Engagement &amp; Consulting
+Interact directly with clients and stakeholders to understand complex business problems.
+Translate business needs into AI/ML opportunities and articulate solution strategies clearly.
+Present solution architectures, effort estimates, timelines, and potential ROI.
+Solution Design &amp; Architecture
+Define end-to-end AI architecture including data pipelines, model selection, AI engines, integration layers, APIs, and deployment strategies.
+Make informed choices of AI/ML/DL algorithms, frameworks, and platforms based on problem type and constraints.
+Ensure the architecture is scalable, modular, secure, and optimized for performance.
+Hands-On Development
+Develop critical components or proof-of-concepts when needed.
+Perform hands-on design and coding for pipelines, model training, inferencing, or integrations.
+Create reusable components and automation scripts for repeatability.
+Team Leadership &amp; Delivery Oversight
+Build and mentor a high-performing AI development team.
+Drive agile development cycles, ensuring timely and quality delivery.
+Collaborate with DevOps, Product Managers, and QA teams throughout SDLC.</t>
+        </is>
+      </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
           <t>AI/ML/DL Expertise:</t>
@@ -593,7 +628,7 @@
       </c>
       <c r="M2" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N2" s="2" t="inlineStr">
@@ -649,7 +684,7 @@
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
@@ -684,7 +719,16 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr"/>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Develop ML and Deep Learning SolutionsCreate predictive, classification, and optimization models using supervised, unsupervised, and reinforcement learning.
+Design and Implement Generative AI SystemsBuild and fine-tune Large Language Models (LLMs) and diffusion models for a range of use cases involving text, code, and multi-modal data.
+Build Scalable Recommendation EnginesDevelop and optimize recommendation systems using collaborative filtering, content-based filtering, hybrid models, or sequential models.
+Cloud-Native ML EngineeringDeploy and manage machine learning pipelines and APIs in cloud environments (AWS, GCP, Azure),ensuring scalability, observability, and cost efficiency.
+End-to-End ML Lifecycle OwnershipOwn the model lifecycle from feature engineering and experimentation to deployment, CI/CD, monitoring, and iteration.
+Collaborate Across FunctionsWork with cross-functional teams including product managers, engineers, and data scientists to translate business goals into AI-powered solutions.</t>
+        </is>
+      </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Languages: Excellent understanding of object-oriented concepts and Python.; ML/DL Frameworks:; Machine Learning: Scikit-learn, XGBoost, LightGBM; Deep Learning: PyTorch, TensorFlow, Keras; GenAI: Hugging Face Transformers, LangChain, OpenAI APIs, Gemini, Agentic Framework; Cloud &amp;amp; MLOps: AWS SageMaker, GCP Vertex AI, Azure ML, MLflow, Kubeflow, Docker, Kubernetes; Data &amp;amp; Compute: Apache Spark, BigQuery, RabbitMQ, S3, EC2; Embedding Stores &amp;amp; Vector Search: FAISS, Pinecone, ChromaDB; Orchestration &amp;amp; APIs: Apache Airflow, Docker Deployment, and FastAPI are a must</t>
@@ -713,7 +757,7 @@
       </c>
       <c r="M4" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N4" s="2" t="inlineStr">
@@ -744,7 +788,20 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>Data mining or extracting usable data from valuable data sources
+Using machine learning tools to select features, create and optimize classifiers
+Carrying out the preprocessing of structured and unstructured data
+Enhancing data collection procedures to include all relevant information for developing analytic systems
+Processing, cleansing, and validating the integrity of data to be used for analysis
+Analyzing large amounts of information to find patterns and solutions
+Developing prediction systems and machine learning algorithms
+Presenting results in a clear manner
+Propose solutions and strategies to tackle business challenges
+Collaborate with Business and IT teams</t>
+        </is>
+      </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
           <t>Programming Skills – knowledge of statistical programming languages like R, Python, and database query languages like SQL, Hive, Pig is desirable. Familiarity with Scala, Java, or C++ is an added advantage.; Statistics – Good applied statistical skills, including knowledge of statistical tests, distributions, regression, maximum likelihood estimators, etc. Proficiency in statistics is essential for data-driven companies.; Machine Learning – good knowledge of machine learning methods like k-Nearest Neighbors, Naive Bayes, SVM, Decision Forests.; Strong Math Skills (Multivariable Calculus and Linear Algebra) – understanding the fundamentals of Multivariable Calculus and Linear Algebra is important as they form the basis of a lot of predictive performance or algorithm optimization techniques.; Data Wrangling – proficiency in handling imperfections in data is an important aspect of a data scientist job description.; Experience with Data Visualization Tools like matplotlib, ggplot, d3.js., Tableau that help to visually encode data; Excellent Communication Skills – it is incredibly important to describe findings to a technical and non-technical audience.; Strong Software Engineering Background; Hands-on experience with data science tools; Problem-solving aptitude; Analytical mind and great business sense; Degree in Computer Science, Engineering or relevant field is preferred; Proven Experience as Data Analyst or Data Scientist</t>
@@ -773,7 +830,7 @@
       </c>
       <c r="M5" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N5" s="2" t="inlineStr">
@@ -833,7 +890,7 @@
       </c>
       <c r="M6" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N6" s="2" t="inlineStr">
@@ -897,7 +954,7 @@
       </c>
       <c r="M7" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N7" s="2" t="inlineStr">
@@ -953,7 +1010,7 @@
       </c>
       <c r="M8" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N8" s="2" t="inlineStr">
@@ -988,7 +1045,21 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr"/>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>The position holder is primarily responsible for revenue generation. through acquisition of new customers and strategic alliances with existing customers.
+Research and identify new business opportunities – including new markets, growth areas, trends, customers, partnerships, products and services.
+Implement effective Sales strategies and contribute to revenue targets.
+Develop a growth strategy focused both on financial gain and customer satisfaction.
+Understand client needs and present appropriate IT solutions to meet their requirements.
+Build strategic alliances, joint ventures or collaborations that create mutually beneficial opportunities.
+Prepare and deliver sales proposals, quotes, and contracts to prospective clients.
+Generate regular reports on sales performance and forecasts.
+Maintain accurate records of sales activities, including sales calls, presentations, and closed deals.
+Work closely with internal teams to develop customized solutions based on client needs.
+Build and maintain strong, long-lasting relationships with clients.</t>
+        </is>
+      </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
           <t>Minimum of 5 years of experience in IT business development.; Proven track record of high value client acquisitions, IT sales with a successful track record.; Deep understanding of the technology industry, technology trends, and emerging technologies.; Exceptional negotiation and communication skills, with the ability to build strong relationships with key stakeholders at all levels of an organization.; Exceptional presales documentation skills.; Ability to translate data and information into actionable insights and business recommendations.; Excellent Time management and planning skills.; Ability to work independently and collaboratively in a team environment.; Results-driven with a focus on achieving and exceeding sales targets.; Responsible for achieving on-boarding targets, sales targets of team as well as individual.; Ability to work independently with strong lead generation skills.; In-depth knowledge of social media marketing, content marketing and brand marketing.; The ability to quickly build rapport and establish meaningful connections with potential clients.</t>
@@ -1013,7 +1084,7 @@
       </c>
       <c r="M9" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N9" s="2" t="inlineStr">
@@ -1048,7 +1119,22 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr"/>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>Collaborate closely with the business team to comprehend project-specific business requirements, fostering effective relationships with clients.
+Define project deliverables, resource needs, and a comprehensive work plan, overseeing their development and successful delivery.
+Guarantee adherence to financial parameters outlined by the business unit throughout the project.
+Coordinate and manage project teams, providing guidance, support, and motivation.
+Engage with stakeholders to gather requirements, provide updates, and manage expectations.
+Oversee the implementation of technical solutions, including code reviews, testing, and deployment.
+Develop accurate project estimates and comprehensive plans, incorporating contingency measures from project initiation to completion.
+Collaborate with the QA team to ensure projects meet stringent quality standards and align with all Techversant processes.
+Effectively manage, monitor, and inspire the assigned project team to achieve optimal performance.
+Conduct compelling project presentations and compile comprehensive reports for stakeholders.
+Facilitate management training sessions to acquaint teams with organizational processes and procedures.
+Proactively identify and report potential risks and issues to management for timely resolution.</t>
+        </is>
+      </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
           <t>Accumulated over 12+ years of experience in the Software Development Industry.; Atleast 3 years of experience as a Tech Lead in any of the technologies like .net, java, javascript etc.; Demonstrated leadership/management roles for single or multiple clients, with a minimum of 10+ years of experience.; Robust technical background in Open Source and Mobile development.; Understanding of AWS, GCP or Azure.; Proficiency in Agile project management.; Solid understanding of current and emerging technologies in the industry.; Strong analytical skills and an aptitude for problem-solving.; Excellent communication and documentation skills.</t>
@@ -1077,7 +1163,7 @@
       </c>
       <c r="M10" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N10" s="2" t="inlineStr">
@@ -1141,7 +1227,7 @@
       </c>
       <c r="M11" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N11" s="2" t="inlineStr">
@@ -1176,7 +1262,18 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr"/>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>Develop and maintain web applications using server-side technologies such as PHP or Python.
+Collaborate with the UI/UX team to implement responsive and user-friendly web interfaces using HTML, CSS, and JavaScript.
+Write clean, efficient, and maintainable code, following OOP (Object-Oriented Programming) principles.
+Troubleshoot, debug, and optimize web applications to ensure maximum performance and usability.
+Assist in designing and implementing new features and functionalities.
+Ensure responsive design and cross-browser compatibility for a seamless user experience across devices.
+Participate in code reviews, providing constructive feedback and learning from senior developers.
+Stay updated with industry trends and continuously improve your knowledge of new technologies and frameworks.</t>
+        </is>
+      </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
           <t>2-3 years of experience in web development, with expertise in server-side technologies such as PHP or Python, and UI development using HTML, CSS, and JavaScript.; Strong understanding of data structures and algorithms.; Proficiency in Object-Oriented Programming (OOP) principles, with practical experience in building scalable and maintainable software.; Strong logical thinking and problem-solving skills, with the ability to break down complex problems into manageable solutions.; Experience with version control tools like Git.; Solid understanding of responsive web design and UI/UX principles.; Experience working with RESTful APIs and integrating web services.; Strong communication skills and the ability to collaborate effectively with cross-functional teams.; Knowledge of databases such as MSSQL, MySQL or PostgreSQL.; A demonstrated willingness to learn new technologies and a passion for continuous self-improvement.</t>
@@ -1205,7 +1302,7 @@
       </c>
       <c r="M12" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N12" s="2" t="inlineStr">
@@ -1240,7 +1337,16 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F13" s="2" t="inlineStr"/>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>Design, implement and support the technical solution.
+Participate actively in all phases of the application development lifecycle.
+Work with user experience designers to ensure all user interactions are
+Implemented correctly and optimized for performance so that we can build an amazing user experience.
+Work within an agile group for varying degrees to deliver solutions.
+You will be responsible for writing server-side web application logic in JavaScript and/or variants of it.</t>
+        </is>
+      </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
           <t>4+ years of experience as developer using Angular.; Experience designing, implementing and using RESTful Web Services.; Experience in Event Driven Programming; Expertise in RXJS; Excellent knowledge on HTML5, CSS3, and cross-browser layout skills and responsive design knowledge.; Attention to detail and an ability to build reliable, scalable, and flexible software.; Ability to work as individual contributor as well as a good team player.; Solid understanding of version control principles, preferably using Git.; Good Communication Skills.; Knowledge and experience with modern JavaScript frameworks and libraries such as AngularJS, React, D3, etc will be an added advantage.</t>
@@ -1269,7 +1375,7 @@
       </c>
       <c r="M13" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N13" s="2" t="inlineStr">
@@ -1304,7 +1410,23 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F14" s="2" t="inlineStr"/>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>Lead a team of developers and provide technical guidance, mentoring, and performance management.
+Lead code reviews to ensure code quality, consistency, and adherence to coding standards.
+Design and develop high-quality software solutions using .NET Core, Angular or React, MS SQl and Azure technologies
+Collaborate with cross-functional teams to understand project requirements and translate them into technical specifications.
+Stay up-to-date with the latest .NET technologies, frameworks, and best practices.
+Troubleshoot and resolve complex technical issues across the application stack.
+Work closely with product managers and designers to ensure successful project delivery.
+Manage and prioritize project tasks, ensuring deadlines are met and milestones achieved.
+Architect scalable and maintainable solutions that align with the company’s technical vision.
+Participate in project planning, estimation, and documentation processes.
+Should take effort to understand the code in other technology project and convert the project into dotnet project, if such requirement comes.
+Ready to learn new technologies.
+Ensures code reviews, unit testing and integration testing is completed efficiently and effectively.</t>
+        </is>
+      </c>
       <c r="G14" s="2" t="inlineStr"/>
       <c r="H14" s="2" t="inlineStr">
         <is>
@@ -1329,7 +1451,7 @@
       </c>
       <c r="M14" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N14" s="2" t="inlineStr">
@@ -1385,7 +1507,7 @@
       </c>
       <c r="M15" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N15" s="2" t="inlineStr">
@@ -1420,7 +1542,18 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F16" s="2" t="inlineStr"/>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>Work closely with team members to support their use of the platform to deliver complete solutions to customers
+Participate in all phases of an agile development cycle – plan, design, implement, review, test, deploy, document, and training
+Troubleshoot and resolve customer issues
+Strive to make continuous improvement
+Architect highly scalable, highly available systems with minimal guidance.
+Translate business requirements into scalable and extensible design.
+Mentor junior engineers on design, coding and troubleshooting.
+Practice and advocate Agile processes in the team</t>
+        </is>
+      </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
           <t>4+ years of web development experience with a minimum of 3 years having hands-on experience using GoLang; Deep understanding of RDBMS; Ability to instill and enforce best practices around web development; A sense of urgency and ownership over the product; Great attitude towards work and people; Strong working knowledge in Golang; Working experience with any of the GoLang Web framework; Strong design skills, awareness of design and architectural patterns; Good understanding of data structures and algorithms; Excellent analytical and problem-solving skills; Ability to work in a fast-paced service environment; Experience in technical mentorship/coaching is highly desirable; Excellent written and verbal communication</t>
@@ -1449,7 +1582,7 @@
       </c>
       <c r="M16" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N16" s="2" t="inlineStr">
@@ -1509,7 +1642,7 @@
       </c>
       <c r="M17" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N17" s="2" t="inlineStr">
@@ -1544,7 +1677,19 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F18" s="2" t="inlineStr"/>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>Lead the development and implementation of mobile applications using React Native.
+Collaborate with cross-functional teams to gather and analyze project requirements.
+Previous ownership of app development projects is required.
+Develop automated tests to guarantee the product’s top-notch quality.
+Stay updated with the latest advancements and changes in mobile platforms and technologies.
+Provide technical supervision and support to mentor the team effectively.
+Conduct code reviews to ensure adherence to coding standards, best practices, and maintain code quality.
+Ensure the application is published and maintained in both the App Store and Google Play Store, adhering to their respective policies and guideline.
+Participate in agile development processes, including sprint planning, estimation, and retrospectives.</t>
+        </is>
+      </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
           <t>7+ years of experience in React Native Development, Minimum 3 yrs in Lead role.; Expert-level proficiency in JavaScript, TypeScript, and React Native framework.; Demonstrated hands-on experience in designing and developing applications using React Native, iOS and Android platforms.; Capability to plan the core architecture and iteratively enhance it as needed.; Strong analytical mindset to extract actionable insights from data.; Excellent Team management and communication skills.; Experience with RESTful APIs and integration of third-party libraries and APIs.; Possess a comprehensive understanding of React Native.; Capable of understanding the company’s business needs and adjusting or innovating the product accordingly.</t>
@@ -1573,7 +1718,7 @@
       </c>
       <c r="M18" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N18" s="2" t="inlineStr">
@@ -1608,7 +1753,22 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F19" s="2" t="inlineStr"/>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>The position holder is primarily responsible for revenue generation. through acquisition of new customers and strategic alliances with existing customers.
+Research and identify new business opportunities – including new markets, growth areas, trends, customers, partnerships, products and services.
+Implement effective Sales strategies and contribute to revenue targets.
+Develop a growth strategy focused both on financial gain and customer satisfaction.
+Understand client needs and present appropriate IT solutions to meet their requirements.
+Build strategic alliances, joint ventures or collaborations that create mutually beneficial opportunities.
+Prepare and deliver sales proposals, quotes, and contracts to prospective clients.
+Generate regular reports on sales performance and forecasts.
+Maintain accurate records of sales activities, including sales calls, presentations, and closed deals.
+Work closely with internal teams to develop customized solutions based on client needs.
+Build and maintain strong, long-lasting relationships with clients.
+Build, lead, mentor, and motivate the business team to achieve sales targets and objectives.</t>
+        </is>
+      </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
           <t>Minimum of 7 years of experience in IT business development.; Proven track record of high value client acquisitions, IT sales with a successful track record.; Deep understanding of the technology industry, technology trends, and emerging technologies.; Exceptional negotiation and communication skills, with the ability to build strong relationships with key stakeholders at all levels of an organization.; Exceptional presales documentation skills.; Ability to translate data and information into actionable insights and business recommendations.; Excellent Time management and planning skills.; Ability to work independently and collaboratively in a team environment.; Results-driven with a focus on achieving and exceeding sales targets.; Responsible for achieving on-boarding targets, sales targets of team as well as individual.; Ability to work independently with strong lead generation skills.; In-depth knowledge of social media marketing, content marketing and brand marketing.; The ability to quickly build rapport and establish meaningful connections with potential clients.; Team building and management skills.</t>
@@ -1637,7 +1797,7 @@
       </c>
       <c r="M19" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N19" s="2" t="inlineStr">
@@ -1672,7 +1832,23 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F20" s="2" t="inlineStr"/>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>Collaborate with cross-functional teams to gather and analyze project requirements, and then translate them into technical specifications and development plans.
+Design and develop responsive and intuitive frontend interfaces using Angular, ensuring seamless user experiences across different devices.
+Create and maintain robust backend APIs and services using Node.js, Express, and related technologies.
+Implement secure authentication and authorization mechanisms for both frontend and backend components.
+Write clean, modular, and efficient code that follows coding standards and best practices.
+Debug and troubleshoot complex issues across the application stack, ensuring optimal performance and reliability.
+Integrate third-party APIs and external services into the applications as needed.
+Work closely with UI/UX Designers to implement visually appealing and user-centric interfaces.
+Collaborate with other developers to conduct code reviews and maintain code quality.
+Mentor and assist junior developers in their technical growth and skill development.
+Stay updated with emerging trends and technologies in full stack development and share insights with the team.
+Experience in relational and non-relation databases and ability to write complex queries.
+Ability to understand business requirement and model it as database entities.</t>
+        </is>
+      </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
           <t>Bachelor’s degree in Computer Science, Engineering, or a related field (or equivalent practical experience); Minimum of 6 years of hands-on experience in full stack development using Angular and Node.js.; Proficiency in TypeScript for frontend development and JavaScript for backend development.; Strong expertise in building responsive single-page applications (SPAs) using Angular, including components, services, and state management.; Experience in developing RESTful APIs and backend services using Node.js, Express, and related technologies.; Familiarity with databases such as MongoDB, MySQL, or PostgreSQL.; Solid understanding of version control systems, especially Git.; Knowledge of frontend build tools and bundlers (e.g., Webpack, Babel).; Strong problem-solving skills and the ability to tackle complex technical challenges.; Excellent teamwork and communication skills.; A portfolio of completed projects showcasing your proficiency in Angular and Node.js development.; Experience with other frontend or backend frameworks is a plus.</t>
@@ -1701,7 +1877,7 @@
       </c>
       <c r="M20" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N20" s="2" t="inlineStr">
@@ -1732,7 +1908,23 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F21" s="2" t="inlineStr"/>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>Experience in Design, Development, and Delivery of large-scale Web Applications.
+Should be competent in code optimization techniques, coding practices and Static code analysis tools.
+Should be competent in understanding complex business requirements.
+Demonstrates the ability to solve problems and create solutions independently.
+Addresses the problems of systems integration, compatibility, and multiple platforms.
+Capable enough to communicate with clients to understand the technical requirements and present technical solutions and system design.
+Ability to analyse the business requirement, prepare work breakdown structure and provide technical estimate.
+Provides good visibility and update on the progress of all activities and tasks, escalating issues and in a timely manner.
+Maintain a cohesive spirit to accomplish the team responsibilities.
+Proficient enough to be a lead contributor on assigned projects.
+Instructs, assigns, directs, and checks the work of other software developers on development team when required.
+Should be able to conduct peer reviews on code quality.
+Need to ensure the Information Security in all perspectives.</t>
+        </is>
+      </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
           <t>8+ years of Work experience as a Senior Java Developer and 2 years in Lead Role.; In-depth knowledge of popular Java frameworks and Spring frameworks (Core/MVC/Spring Boot etc.); Proficient knowledge and experience in Webservices (REST/SOAP).; Strong knowledge in writing stored procedures and SQL queries.; Experience in modelling databases based on various business requirements.; Strong knowledge in Data Analysis.; Proficiency in Angular or similar frontend frameworks is desirable.; Working experience with GIT and Artefactory.; Good knowledge of DevOps, Test Driven Development and CI/CD pipelines is desirable.; Deployment to Cloud Services.</t>
@@ -1761,7 +1953,7 @@
       </c>
       <c r="M21" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N21" s="2" t="inlineStr">
@@ -1796,7 +1988,27 @@
           <t>Posted on 23.07.2025</t>
         </is>
       </c>
-      <c r="F22" s="2" t="inlineStr"/>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>Mentor junior members of the team.
+Provide timely code reviews for peers.
+Develop high-quality software solutions using .NET Core, Angular or React, MS SQl and Azure technologies
+Collaborate with cross-functional teams to understand project requirements and translate them into technical specifications.
+Stay up-to-date with the latest .NET technologies, frameworks, and best practices.
+Troubleshoot and resolve complex technical issues across the application stack.
+Actively participates in scrum meetings and analyzes requirements to understand technical/functional requirements. Also possess a capability to discuss requirement with client directly.
+Ability to work as an individual contributor.
+Ability to assign task to junior members of the team and guide them in their development
+Manage and prioritize project tasks after discussing with client, ensuring deadlines are met and milestones achieved.
+Participate in project planning, estimation, and documentation processes.
+Should take effort to understand the code in other technology project and convert the project into dotnet project, if such requirement comes.
+Ready to learn new technologies.
+Should have a commitment to complete the task on time without a follow up from senior.
+Learn technology business domain and system domain as recommended by the project
+Code ,debug,test , document and communicate product/component/feature development stage
+Ensures code reviews, unit testing and integration testing is completed efficiently and effectively.</t>
+        </is>
+      </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
           <t>Bachelor’s degree in Computer Science, Engineering, or a related field (or equivalent practical experience; Minimum 5+ years of experience in the dotnet technology.; Fluent in English.; Proficiency in .NET Core, C#, NET MVC, Web API.; Strong expertise in frontend technologies including Angular or React, TypeScript, HTML, CSS and JavaScript.; Experience in cloud technologies, particularly Azure services (e.g., Azure App Service, Azure Functions).; Knowledge in the Azure Devops will add more value to the role.; Excellent problem-solving skills and the ability to troubleshoot complex technical challenges.; Strong communication skills and the ability to collaborate effectively with cross-functional teams.; Familiarity with version control systems, especially Git.; Proven ability to work as an individual contributor.; Experience with Agile methodologies like scrum and practices is a plus.</t>
@@ -1821,7 +2033,7 @@
       </c>
       <c r="M22" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N22" s="2" t="inlineStr">
@@ -1881,7 +2093,7 @@
       </c>
       <c r="M23" s="2" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:02</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
       <c r="N23" s="2" t="inlineStr">
@@ -1943,7 +2155,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-02 06:58:03</t>
+          <t>2025-08-03 21:19:22</t>
         </is>
       </c>
     </row>

</xml_diff>